<commit_message>
efficiency residuals for optimal energy windows at low activities calculated
</commit_message>
<xml_diff>
--- a/efficiency/set_4/data/HidexAMG-Track_30min-035-20240501-184615-AutoExport.xlsx
+++ b/efficiency/set_4/data/HidexAMG-Track_30min-035-20240501-184615-AutoExport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuliy\OneDrive\Documents\Fall 2023\Research\efficiency\set_4\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D409D5-BC24-45BD-8947-6AD510B6253E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7AA107-812F-431C-B62E-F0C2BDC7517F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>

</xml_diff>